<commit_message>
Fixed JV budget check for contra entry and added BudgetAutoUpdate methods.
</commit_message>
<xml_diff>
--- a/vcm/erpnext_vcm/testing/excelfiles/Budget-Ramnavami.xlsx
+++ b/vcm/erpnext_vcm/testing/excelfiles/Budget-Ramnavami.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="37">
   <si>
     <t>Company</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>RAM NAVAMI - HKMV</t>
+  </si>
+  <si>
+    <t>Deity Pooja</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Unlinked Payments</t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
   <dimension ref="A1:F3045"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -803,6 +812,9 @@
       <c r="E13" t="s">
         <v>5</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -840,6 +852,9 @@
       <c r="E15" t="s">
         <v>5</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -857,6 +872,9 @@
       <c r="E16" t="s">
         <v>5</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
@@ -914,6 +932,9 @@
       <c r="E19" t="s">
         <v>5</v>
       </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
@@ -931,6 +952,9 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
@@ -948,6 +972,9 @@
       <c r="E21" t="s">
         <v>5</v>
       </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
@@ -965,6 +992,9 @@
       <c r="E22" t="s">
         <v>5</v>
       </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -982,6 +1012,9 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
@@ -1018,6 +1051,69 @@
       </c>
       <c r="E25" t="s">
         <v>5</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="1927" spans="6:6">

</xml_diff>